<commit_message>
Actualizando documentos de pruebas
</commit_message>
<xml_diff>
--- a/Deliverables/4) Verification/Black_Box_Tests.xlsx
+++ b/Deliverables/4) Verification/Black_Box_Tests.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Black_Box_TP-1" sheetId="1" r:id="rId1"/>
     <sheet name="Black_Box_TP-2" sheetId="2" r:id="rId2"/>
     <sheet name="Black_Box_TP-3" sheetId="4" r:id="rId3"/>
+    <sheet name="Black_Box_TP-4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>Test ID</t>
   </si>
@@ -48,9 +49,6 @@
     <t>2. Position the multimeter tips at the output of the power source powering the motor</t>
   </si>
   <si>
-    <t>The measured voltage is equal to 12 VCD with a tolerance of (xx)</t>
-  </si>
-  <si>
     <t>Actual  Results</t>
   </si>
   <si>
@@ -69,182 +67,6 @@
     <t>1. Turn on the motor</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">3. Verify that the measured voltage is equal to 12 VCD with a tolerance of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(xx)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4. Position the multimeter tips at </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>xx pins of xx circuit.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Verify that the measured voltage is equal to 12 VCD with a tolerance of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(xx)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The measured voltage is equal to 12 VCD with a tolerance of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(xx)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2. Press the button called "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Diagnosticos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" in the LCD screen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3. Verify that there is a change of screen. The LCD screen should be showing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the diagnoses</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4. Press the button called </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Desempeño" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in the LCD screen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Verify that there is a change of screen. The LCD screen should be showing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the performance status</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There is a change of screen. The LCD screen is showing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the performance status</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There is a change of screen. The LCD screen is showing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the diagnoses</t>
-    </r>
-  </si>
-  <si>
     <t>6. Verify that the screen is showing the following:</t>
   </si>
   <si>
@@ -281,15 +103,9 @@
     <t>DSE-117, DSE-92, DSE-116, DSE-95</t>
   </si>
   <si>
-    <t>3. Verify that the screen has enough constrat and lightning for the data written on it to be read.</t>
-  </si>
-  <si>
     <t>DSE-95</t>
   </si>
   <si>
-    <t>The data on the screen can be read</t>
-  </si>
-  <si>
     <t>The screen is not blinking</t>
   </si>
   <si>
@@ -318,6 +134,99 @@
   </si>
   <si>
     <t>Black_Box_TP-3</t>
+  </si>
+  <si>
+    <t>DSE_SW-8</t>
+  </si>
+  <si>
+    <t>1. Oscilloscope</t>
+  </si>
+  <si>
+    <t>CH1 +</t>
+  </si>
+  <si>
+    <t>CH1-</t>
+  </si>
+  <si>
+    <t>1. Turn on the oscilloscope</t>
+  </si>
+  <si>
+    <t>2. Set the oscilloscope as follows:</t>
+  </si>
+  <si>
+    <t>5 V</t>
+  </si>
+  <si>
+    <t>100 ms</t>
+  </si>
+  <si>
+    <t>Edge Trigger</t>
+  </si>
+  <si>
+    <t>3. Press the Run/Stop button in the oscilloscope and ensure the trigger is ready</t>
+  </si>
+  <si>
+    <t>3. Turn on the motor</t>
+  </si>
+  <si>
+    <t>4. Wait for the oscilloscope to stop</t>
+  </si>
+  <si>
+    <t>4. Position the multimeter tips at V+ and GND pins of H-bridge circuit.</t>
+  </si>
+  <si>
+    <t>3. Verify that the screen header is Control Vel. Motor CD, this means the screen has good constrat and lightning.</t>
+  </si>
+  <si>
+    <t>The screen header is Control Vel.Motor CD</t>
+  </si>
+  <si>
+    <t>3. Verify that there is a change of screen. The LCD screen should be showing the diagnoses</t>
+  </si>
+  <si>
+    <t>2. Press the button called "Ver Diagnosticos" on the LCD screen</t>
+  </si>
+  <si>
+    <t>4. Press the button called "Regresar" on the LCD screen</t>
+  </si>
+  <si>
+    <t>5. Verify that there is a change of screen. The LCD screen should be showing the performance status</t>
+  </si>
+  <si>
+    <t>There is a change of screen. The LCD screen is showing the diagnoses</t>
+  </si>
+  <si>
+    <t>There is a change of screen. The LCD screen is showing the performance status</t>
+  </si>
+  <si>
+    <t>Black_Box_TP-4</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Pin 60</t>
+  </si>
+  <si>
+    <t>The measured voltage is equal to 12 VCD with a tolerance of 10%</t>
+  </si>
+  <si>
+    <t>3. Verify that the measured voltage is equal to 12 VCD with a tolerance of +- 0.5V</t>
+  </si>
+  <si>
+    <t>5. Verify that the measured voltage is equal to 12 VCD with a tolerance of +- 0.5V</t>
+  </si>
+  <si>
+    <t>The measured voltage is equal to 12 VCD with a tolerance of +- 0.5V</t>
+  </si>
+  <si>
+    <t>The measured voltage is equal to 12 VCD with a tolerance of +-0.5V</t>
+  </si>
+  <si>
+    <t>5. Verify that the pulse width of channel 1 is equal to 300 ms with a tolerance of +- 50 ms</t>
+  </si>
+  <si>
+    <t>The pulse width of channel 1 is equal to 300 ms with a tolerance of +- 50 ms</t>
   </si>
 </sst>
 </file>
@@ -333,24 +242,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -361,8 +255,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,6 +290,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -394,22 +309,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,15 +651,16 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -745,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -753,73 +676,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,29 +753,32 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>13</v>
+      <c r="A22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>13</v>
+      <c r="A23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -866,10 +795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,15 +807,16 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -894,214 +824,206 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
+      <c r="A17" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="13"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="4"/>
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>31</v>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="1" t="s">
-        <v>30</v>
+      <c r="A33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="4"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="F42" s="8"/>
+      <c r="A37" s="4"/>
+      <c r="F37" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,84 +1053,249 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B14" s="13"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="F22" s="8"/>
+      <c r="A18" s="4"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="F19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="14"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>